<commit_message>
Added Validation Logic -check if master file is alright
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alen\Documents\UI Path Projects\BRIT_RPDOrderForm\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90410B63-B5AE-480F-906B-170C5646EE7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913FC4B-68E6-4766-B21F-3787192B14F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34200" yWindow="2640" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32220" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
     <t>Sheet1</t>
   </si>
   <si>
-    <t>Sheet name ti the master file</t>
+    <t>Sheet name to the master file</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Added process name in the config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alen\Documents\UI Path Projects\BRIT_RPDOrderForm\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913FC4B-68E6-4766-B21F-3787192B14F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B428AC1-9B25-4AD8-AE13-DC846F0C03D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32220" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32220" yWindow="2535" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Sheet name to the master file</t>
+  </si>
+  <si>
+    <t>BRIT_RPDOrderForm</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -585,13 +585,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -600,45 +600,45 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="str">
         <f>_xlfn.CONCAT(B6,"\","Master File\AW Master.xlsx")</f>
         <v>C:\Users\Alen\Documents\RPD Processing Folder\Master File\AW Master.xlsx</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1693,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1717,7 +1717,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1739,7 +1739,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1750,7 +1750,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1761,7 +1761,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2799,13 +2799,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>